<commit_message>
[OBC] Added updated excel export
</commit_message>
<xml_diff>
--- a/bus/obc/Project Outputs for obc/obc_v4.3_BOM.xlsx
+++ b/bus/obc/Project Outputs for obc/obc_v4.3_BOM.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0625AC03-1AB2-4B85-BBAB-BC981F5AE163}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D97E662D-F7F2-44D8-BF58-6A03FF5932B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="975" windowWidth="13680" windowHeight="12105" xr2:uid="{BA002BC9-BA4A-4881-AF9D-8723E1C89305}"/>
+    <workbookView xWindow="675" yWindow="975" windowWidth="13680" windowHeight="12105" xr2:uid="{18021BBB-4A92-4235-8298-79B9CFD9A135}"/>
   </bookViews>
   <sheets>
-    <sheet name="obc_v4.3_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="obc_4.3.1_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="141">
   <si>
     <t>Line #</t>
   </si>
@@ -82,6 +82,24 @@
     <t>0402 capacitor</t>
   </si>
   <si>
+    <t>C1_FLASH1, C1_FLASH2, C1_FLASH3, C2, C3, C4, C37, C44, C46, C47, C48</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>Manual Solution</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>311-0.0JRCT-ND</t>
+  </si>
+  <si>
     <t>C38</t>
   </si>
   <si>
@@ -94,9 +112,6 @@
     <t>Volume Production</t>
   </si>
   <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
     <t>399-17558-1-ND</t>
   </si>
   <si>
@@ -115,6 +130,27 @@
     <t>0402 resistor</t>
   </si>
   <si>
+    <t>R1_FLASH1, R1_FLASH2, R1_FLASH3, R2, R3, R4, R5, R7, R8, R10, R28, R29, R65</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1002X</t>
+  </si>
+  <si>
+    <t>P10.0KLCT-ND</t>
+  </si>
+  <si>
+    <t>R26, R27, R50, R51, R52</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1000X</t>
+  </si>
+  <si>
+    <t>P100LCT-ND</t>
+  </si>
+  <si>
     <t>R49, R53</t>
   </si>
   <si>
@@ -130,9 +166,6 @@
     <t>R54, R55</t>
   </si>
   <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
     <t>ERJ-2GE0R00X</t>
   </si>
   <si>
@@ -163,9 +196,6 @@
     <t>R72</t>
   </si>
   <si>
-    <t>Yageo</t>
-  </si>
-  <si>
     <t>AC0402FR-0730KL</t>
   </si>
   <si>
@@ -244,6 +274,156 @@
     <t>ATMEGA64M1-AU-ND</t>
   </si>
   <si>
+    <t>DS3234</t>
+  </si>
+  <si>
+    <t>SPI bus RTC with integrated crystal and SRAM</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>Maxim</t>
+  </si>
+  <si>
+    <t>DS3234SN#T&amp;R</t>
+  </si>
+  <si>
+    <t>DS3234SN#T&amp;RCT-ND</t>
+  </si>
+  <si>
+    <t>SC18IS600IPW/S8HP</t>
+  </si>
+  <si>
+    <t>SPI to I2C bridge.</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>NXP USA</t>
+  </si>
+  <si>
+    <t>568-13690-1-ND</t>
+  </si>
+  <si>
+    <t>SLW-102-01-G-D</t>
+  </si>
+  <si>
+    <t>4 pos 100mil pitch low profile header</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>SAM1088-02-ND</t>
+  </si>
+  <si>
+    <t>SLW-103-01-G-D</t>
+  </si>
+  <si>
+    <t>6 pos 100mil pitch low profile header</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>SAM1088-03-ND</t>
+  </si>
+  <si>
+    <t>SLW-115-01-G-S</t>
+  </si>
+  <si>
+    <t>15 Position Receptacle Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>SAM1089-15-ND</t>
+  </si>
+  <si>
+    <t>SN65HVD233D</t>
+  </si>
+  <si>
+    <t>3.3V CAN Transceiver with Standby Mode, Loop-back 8-SOIC -40 to 125</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>296-14639-5-ND</t>
+  </si>
+  <si>
+    <t>SN74HC365PW</t>
+  </si>
+  <si>
+    <t>Hex non-inverting buffer with 3-state outputs</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>296-33932-5-ND</t>
+  </si>
+  <si>
+    <t>SN74LVC1G07</t>
+  </si>
+  <si>
+    <t>Single element non-inverting open drain buffer</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SN74LVC1G07DCKR</t>
+  </si>
+  <si>
+    <t>296-8486-1-ND</t>
+  </si>
+  <si>
+    <t>SST26VF016B</t>
+  </si>
+  <si>
+    <t>2.5V/3.0V 16 Mbit Serial Quad I/O (SQI) Flash Memory</t>
+  </si>
+  <si>
+    <t>U1_FLASH1, U1_FLASH2, U1_FLASH3</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>SST26VF016B-104I/SN</t>
+  </si>
+  <si>
+    <t>SST26VF016B-104I/SN-ND</t>
+  </si>
+  <si>
+    <t>SW-PB</t>
+  </si>
+  <si>
+    <t>Schematic symbol for a generic 2-pin pushbutton, OFF-mom.</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>ITT C&amp;K</t>
+  </si>
+  <si>
+    <t>PTS830GM140SMTRLFS</t>
+  </si>
+  <si>
+    <t>CKN10587CT-ND</t>
+  </si>
+  <si>
     <t>DPDT</t>
   </si>
   <si>
@@ -253,160 +433,13 @@
     <t>S1</t>
   </si>
   <si>
-    <t>ITT C&amp;K</t>
-  </si>
-  <si>
     <t>JS202011AQN</t>
   </si>
   <si>
-    <t>401-2000-ND</t>
-  </si>
-  <si>
-    <t>DS3234</t>
-  </si>
-  <si>
-    <t>SPI bus RTC with integrated crystal and SRAM</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>Maxim</t>
-  </si>
-  <si>
-    <t>DS3234SN#T&amp;R</t>
-  </si>
-  <si>
-    <t>DS3234SN#T&amp;RCT-ND</t>
-  </si>
-  <si>
-    <t>SC18IS600IPW/S8HP</t>
-  </si>
-  <si>
-    <t>SPI to I2C bridge.</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>NXP USA</t>
-  </si>
-  <si>
-    <t>568-13690-1-ND</t>
-  </si>
-  <si>
-    <t>SLW-102-01-G-D</t>
-  </si>
-  <si>
-    <t>4 pos 100mil pitch low profile header</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>SAM1088-02-ND</t>
-  </si>
-  <si>
-    <t>SLW-103-01-G-D</t>
-  </si>
-  <si>
-    <t>6 pos 100mil pitch low profile header</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>SAM1088-03-ND</t>
-  </si>
-  <si>
-    <t>SLW-115-01-G-S</t>
-  </si>
-  <si>
-    <t>15 Position Receptacle Connector 0.100" (2.54mm) Through Hole Gold</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>SAM1089-15-ND</t>
-  </si>
-  <si>
-    <t>SN65HVD233D</t>
-  </si>
-  <si>
-    <t>3.3V CAN Transceiver with Standby Mode, Loop-back 8-SOIC -40 to 125</t>
-  </si>
-  <si>
-    <t>U14</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>296-14639-5-ND</t>
-  </si>
-  <si>
-    <t>SN74HC365PW</t>
-  </si>
-  <si>
-    <t>Hex non-inverting buffer with 3-state outputs</t>
-  </si>
-  <si>
-    <t>U17</t>
-  </si>
-  <si>
-    <t>296-33932-5-ND</t>
-  </si>
-  <si>
-    <t>SN74LVC1G07</t>
-  </si>
-  <si>
-    <t>Single element non-inverting open drain buffer</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SN74LVC1G07DCKR</t>
-  </si>
-  <si>
-    <t>296-8486-1-ND</t>
-  </si>
-  <si>
-    <t>SST26VF016B</t>
-  </si>
-  <si>
-    <t>2.5V/3.0V 16 Mbit Serial Quad I/O (SQI) Flash Memory</t>
-  </si>
-  <si>
-    <t>U1_FLASH1, U1_FLASH2, U1_FLASH3</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>SST26VF016B-104I/SN</t>
-  </si>
-  <si>
-    <t>SST26VF016B-104I/SN-ND</t>
-  </si>
-  <si>
-    <t>SW-PB</t>
-  </si>
-  <si>
-    <t>Schematic symbol for a generic 2-pin pushbutton, OFF-mom.</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>PTS830GM140SMTRLFS</t>
-  </si>
-  <si>
-    <t>CKN10587CT-ND</t>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>611-JS202011AQN</t>
   </si>
   <si>
     <t>SLH-010-1.50-G-D-A</t>
@@ -416,27 +449,6 @@
   </si>
   <si>
     <t>J4</t>
-  </si>
-  <si>
-    <t>C1_FLASH1, C1_FLASH2, C1_FLASH3, C2, C3, C4, C37, C44, C46, C47, C48</t>
-  </si>
-  <si>
-    <t>[NoParam], Digi-Key</t>
-  </si>
-  <si>
-    <t>[NoParam], 587-3807-1-ND</t>
-  </si>
-  <si>
-    <t>R1_FLASH1, R1_FLASH2, R1_FLASH3, R2, R3, R4, R5, R7, R8, R10, R28, R29, R65</t>
-  </si>
-  <si>
-    <t>[NoParam], P10.0KLCT-ND</t>
-  </si>
-  <si>
-    <t>R26, R27, R50, R51, R52</t>
-  </si>
-  <si>
-    <t>[NoParam], 541-100YCT-ND</t>
   </si>
 </sst>
 </file>
@@ -830,7 +842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CD1B1C-9FAC-4C19-BF38-9DE71114CBE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CFCADF-99A2-40EA-8289-46043548C4EA}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -937,7 +949,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -955,10 +967,10 @@
         <v>23</v>
       </c>
       <c r="K3" s="3">
-        <v>0.17333000000000001</v>
+        <v>1.9869999999999999E-2</v>
       </c>
       <c r="L3" s="3">
-        <v>0.17333000000000001</v>
+        <v>0.21856999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -975,28 +987,28 @@
         <v>24</v>
       </c>
       <c r="E4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K4" s="3">
-        <v>0.25333</v>
+        <v>0.17224</v>
       </c>
       <c r="L4" s="3">
-        <v>0.50666</v>
+        <v>0.17224</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1007,7 +1019,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>29</v>
@@ -1016,13 +1028,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>22</v>
@@ -1031,10 +1043,10 @@
         <v>32</v>
       </c>
       <c r="K5" s="3">
-        <v>0.13333</v>
+        <v>0.25173000000000001</v>
       </c>
       <c r="L5" s="3">
-        <v>0.26666000000000001</v>
+        <v>0.50346000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1045,19 +1057,19 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
@@ -1066,13 +1078,13 @@
         <v>22</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K6" s="3">
-        <v>0.13333</v>
+        <v>5.9619999999999999E-2</v>
       </c>
       <c r="L6" s="3">
-        <v>0.26666000000000001</v>
+        <v>0.77505999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1083,19 +1095,19 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
@@ -1104,13 +1116,13 @@
         <v>22</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K7" s="3">
-        <v>0.59999000000000002</v>
+        <v>5.9619999999999999E-2</v>
       </c>
       <c r="L7" s="3">
-        <v>1.2</v>
+        <v>0.59619999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1121,34 +1133,34 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K8" s="3">
-        <v>2.9329999999999998E-2</v>
+        <v>0.13249</v>
       </c>
       <c r="L8" s="3">
-        <v>0.29332999999999998</v>
+        <v>0.26497999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1159,22 +1171,22 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>22</v>
@@ -1183,10 +1195,10 @@
         <v>47</v>
       </c>
       <c r="K9" s="3">
-        <v>0.13333</v>
+        <v>0.13249</v>
       </c>
       <c r="L9" s="3">
-        <v>0.13333</v>
+        <v>0.26497999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1194,37 +1206,37 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="K10" s="3">
-        <v>0.29332999999999998</v>
+        <v>0.59619999999999995</v>
       </c>
       <c r="L10" s="3">
-        <v>0.29332999999999998</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1232,37 +1244,37 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="K11" s="3">
-        <v>0.55998999999999999</v>
+        <v>2.9149999999999999E-2</v>
       </c>
       <c r="L11" s="3">
-        <v>1.1200000000000001</v>
+        <v>0.29148000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1270,37 +1282,37 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K12" s="3">
-        <v>1.52</v>
+        <v>0.13249</v>
       </c>
       <c r="L12" s="3">
-        <v>1.52</v>
+        <v>0.13249</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1308,37 +1320,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K13" s="3">
-        <v>7.16</v>
+        <v>0.29148000000000002</v>
       </c>
       <c r="L13" s="3">
-        <v>7.16</v>
+        <v>0.29148000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1346,71 +1358,75 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.55645999999999995</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1.1100000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K15" s="3">
-        <v>11.32</v>
+        <v>1.51</v>
       </c>
       <c r="L15" s="3">
-        <v>11.32</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1418,37 +1434,37 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="K16" s="3">
-        <v>4.08</v>
+        <v>7.11</v>
       </c>
       <c r="L16" s="3">
-        <v>4.08</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1456,37 +1472,37 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="K17" s="3">
-        <v>1.03</v>
+        <v>11.25</v>
       </c>
       <c r="L17" s="3">
-        <v>1.03</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1494,181 +1510,181 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="3">
+        <v>4.05</v>
+      </c>
+      <c r="L18" s="3">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1.02</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K20" s="3">
-        <v>4.17</v>
-      </c>
-      <c r="L20" s="3">
-        <v>4.17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0.89332</v>
-      </c>
-      <c r="L21" s="3">
-        <v>0.89332</v>
-      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K22" s="3">
-        <v>0.57332000000000005</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="L22" s="3">
-        <v>0.57332000000000005</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1676,37 +1692,37 @@
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E23" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K23" s="3">
-        <v>1.59</v>
+        <v>0.88768000000000002</v>
       </c>
       <c r="L23" s="3">
-        <v>4.76</v>
+        <v>0.88768000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1714,37 +1730,37 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="K24" s="3">
-        <v>0.67998999999999998</v>
+        <v>0.43722</v>
       </c>
       <c r="L24" s="3">
-        <v>0.67998999999999998</v>
+        <v>0.43722</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
@@ -1752,118 +1768,130 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1.58</v>
+      </c>
+      <c r="L25" s="3">
+        <v>4.7300000000000004</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="3">
-        <v>11</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="H26" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="K26" s="3">
+        <v>0.67569999999999997</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.67569999999999997</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E27" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.59619999999999995</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.59619999999999995</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E28" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1875,99 +1903,99 @@
         <v>12</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" tooltip="Component" display="'" xr:uid="{56F8F28D-93BB-4DF7-9313-AE2323093CB0}"/>
-    <hyperlink ref="G2" tooltip="Manufacturer" display="'" xr:uid="{9C5D49DE-6A0A-4022-9897-9EE7DDCBA863}"/>
-    <hyperlink ref="J2" tooltip="Supplier" display="'" xr:uid="{6928B0EF-50DF-4DE1-BA67-1393715DEA08}"/>
-    <hyperlink ref="F3" r:id="rId1" tooltip="Component" display="'KEMET" xr:uid="{5047A1C0-81C7-4707-BF85-57F0806AB24F}"/>
-    <hyperlink ref="G3" r:id="rId2" tooltip="Manufacturer" display="'C0402C470J3RACAUTO" xr:uid="{9A7D1F81-2A8C-4ED5-BBE8-75C6412A7B8E}"/>
-    <hyperlink ref="J3" r:id="rId3" tooltip="Supplier" display="'399-17558-1-ND" xr:uid="{2E163848-7BDB-4CD8-B896-A02DE466AD70}"/>
-    <hyperlink ref="F4" r:id="rId4" tooltip="Component" display="'KEMET" xr:uid="{B4545B76-6B2F-4180-AF8E-A3220E4FEBFB}"/>
-    <hyperlink ref="G4" r:id="rId5" tooltip="Manufacturer" display="'C0402C220K4RAC7867" xr:uid="{F86A95A3-FF4F-4556-9B53-840D38ABA169}"/>
-    <hyperlink ref="J4" r:id="rId6" tooltip="Supplier" display="'399-17554-1-ND" xr:uid="{7358A981-E548-4AB0-B779-F57CEB5E3863}"/>
-    <hyperlink ref="F5" r:id="rId7" tooltip="Component" display="'Vishay" xr:uid="{BE5E04E7-44D1-4C0F-BAAC-E848060CAF9A}"/>
-    <hyperlink ref="G5" r:id="rId8" tooltip="Manufacturer" display="'CRCW040260R4FKED" xr:uid="{DB8EE49F-A4D3-4A8C-ABAD-94C7B836221F}"/>
-    <hyperlink ref="J5" r:id="rId9" tooltip="Supplier" display="'541-60.4LCT-ND" xr:uid="{23B0EF5A-EAFA-4E12-9AE3-2F36A59D898E}"/>
-    <hyperlink ref="F6" r:id="rId10" tooltip="Component" display="'Panasonic" xr:uid="{A41AD633-55C6-493B-9317-070FF528179C}"/>
-    <hyperlink ref="G6" r:id="rId11" tooltip="Manufacturer" display="'ERJ-2GE0R00X" xr:uid="{36BA6701-3217-4D60-B6BD-F3C64922BD51}"/>
-    <hyperlink ref="J6" r:id="rId12" tooltip="Supplier" display="'P0.0JCT-ND" xr:uid="{254C5EB1-8286-4A47-8681-3B77AB9211BC}"/>
-    <hyperlink ref="F7" r:id="rId13" tooltip="Component" display="'Panasonic" xr:uid="{5BA4973B-379F-4089-82CA-129019F22F62}"/>
-    <hyperlink ref="G7" r:id="rId14" tooltip="Manufacturer" display="'ERA-2AEB472X" xr:uid="{0718E7EC-A3CC-405C-B457-C1EA4C7B0A20}"/>
-    <hyperlink ref="J7" r:id="rId15" tooltip="Supplier" display="'P4.7KDCCT-ND" xr:uid="{CC9B7982-3EAD-4E61-A94A-DFE5FD194BE7}"/>
-    <hyperlink ref="F8" r:id="rId16" tooltip="Component" display="'TE Connectivity" xr:uid="{83BC7CBD-E039-4AE2-B132-25109EB4312D}"/>
-    <hyperlink ref="G8" r:id="rId17" tooltip="Manufacturer" display="'CRGCQ0402F330R" xr:uid="{26EBEBD8-3C7F-4981-BF42-825C6AF872B3}"/>
-    <hyperlink ref="J8" r:id="rId18" tooltip="Supplier" display="'A129621CT-ND" xr:uid="{B1B1B37B-6EA8-4B18-B10D-EFE0A6A74D89}"/>
-    <hyperlink ref="F9" r:id="rId19" tooltip="Component" display="'Yageo" xr:uid="{61F23145-654D-4A7C-814F-E5061806FC99}"/>
-    <hyperlink ref="G9" r:id="rId20" tooltip="Manufacturer" display="'AC0402FR-0730KL" xr:uid="{2E4E5A09-0234-4D30-8CF2-2175B8E68633}"/>
-    <hyperlink ref="J9" r:id="rId21" tooltip="Supplier" display="'YAG3474CT-ND" xr:uid="{9B53401B-25F5-4D0C-BC1C-36F52D151572}"/>
-    <hyperlink ref="F10" r:id="rId22" tooltip="Component" display="'TDK" xr:uid="{9AE66092-6633-4E24-AE49-69AB65C7CA5C}"/>
-    <hyperlink ref="G10" r:id="rId23" tooltip="Manufacturer" display="'MLZ1608N100LTD25" xr:uid="{65D5E873-489C-4A64-ACDE-9A01F3EBB8F3}"/>
-    <hyperlink ref="J10" r:id="rId24" tooltip="Supplier" display="'445-17067-1-ND" xr:uid="{BE70D4BB-16C9-4EF7-9C50-350B86698785}"/>
-    <hyperlink ref="F11" r:id="rId25" tooltip="Component" display="'Murata" xr:uid="{5C259B40-9910-493A-A0C4-F957CEE5683C}"/>
-    <hyperlink ref="G11" r:id="rId26" tooltip="Manufacturer" display="'GCM21BR70J106KE22K" xr:uid="{9A1DC030-C4C6-4088-92FA-A361F8BFF0BE}"/>
-    <hyperlink ref="J11" r:id="rId27" tooltip="Supplier" display="'490-14361-1-ND" xr:uid="{C4D49D87-1F06-41E9-91F0-8CC24FFFB348}"/>
-    <hyperlink ref="F12" r:id="rId28" tooltip="Component" display="'Abracon" xr:uid="{38935A8A-3BAA-4967-90C1-CC77892F0A72}"/>
-    <hyperlink ref="G12" r:id="rId29" tooltip="Manufacturer" display="'ABM3B-8.000MHZ-10-D-1-G-T" xr:uid="{8BE5958E-138A-40B3-B4D2-30A7ED82364B}"/>
-    <hyperlink ref="J12" r:id="rId30" tooltip="Supplier" display="'535-13456-1-ND" xr:uid="{7ACAEF93-2F8C-43A1-8A09-37229679A853}"/>
-    <hyperlink ref="F13" r:id="rId31" tooltip="Component" display="'Microchip / Atmel" xr:uid="{7E8E4FF4-48B0-4041-BCFE-010190052372}"/>
-    <hyperlink ref="G13" r:id="rId32" tooltip="Manufacturer" display="'ATMEGA64M1-AU" xr:uid="{4E2E7591-C582-4D63-A9EF-152FB79C824A}"/>
-    <hyperlink ref="J13" r:id="rId33" tooltip="Supplier" display="'ATMEGA64M1-AU-ND" xr:uid="{1AFA8A06-4C48-42BC-92D7-496F13AB1BE8}"/>
-    <hyperlink ref="F14" r:id="rId34" tooltip="Component" display="'ITT C&amp;K" xr:uid="{4623F110-5089-4EC5-855A-352FB7B326EC}"/>
-    <hyperlink ref="G14" r:id="rId35" tooltip="Manufacturer" display="'JS202011AQN" xr:uid="{6DFEB7BE-BE68-441E-82D4-EE515D7CFF99}"/>
-    <hyperlink ref="J14" r:id="rId36" tooltip="Supplier" display="'401-2000-ND" xr:uid="{C701075E-D799-4A0A-827A-A8B4ED62E7D4}"/>
-    <hyperlink ref="F15" r:id="rId37" tooltip="Component" display="'Maxim" xr:uid="{01DA11FB-2CA9-41E6-BB6A-729711718881}"/>
-    <hyperlink ref="G15" r:id="rId38" tooltip="Manufacturer" display="'DS3234SN#T&amp;R" xr:uid="{F3FF9E60-EFE2-47FB-BC14-88B32CE928B2}"/>
-    <hyperlink ref="J15" r:id="rId39" tooltip="Supplier" display="'DS3234SN#T&amp;RCT-ND" xr:uid="{FDA4646A-98BB-4DEF-A45C-6F5DB578A566}"/>
-    <hyperlink ref="F16" r:id="rId40" tooltip="Component" display="'NXP USA" xr:uid="{F9FABD1C-DE06-4EBF-AF72-23BDDD6B61B2}"/>
-    <hyperlink ref="G16" r:id="rId41" tooltip="Manufacturer" display="'SC18IS600IPW/S8HP" xr:uid="{F427E8A7-FA48-432E-8C54-13541F966237}"/>
-    <hyperlink ref="J16" r:id="rId42" tooltip="Supplier" display="'568-13690-1-ND" xr:uid="{67AE5C0C-67DB-4221-807C-928D475D17DB}"/>
-    <hyperlink ref="F17" r:id="rId43" tooltip="Component" display="'Samtec" xr:uid="{9C7647F7-B3D1-479A-81D9-C0379F50347D}"/>
-    <hyperlink ref="G17" r:id="rId44" tooltip="Manufacturer" display="'SLW-102-01-G-D" xr:uid="{31F1918E-2347-4B75-AF3F-744EC5D97756}"/>
-    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'SAM1088-02-ND" xr:uid="{E45D4342-E897-454A-B510-752934D8496D}"/>
-    <hyperlink ref="F18" r:id="rId46" tooltip="Component" display="'Samtec" xr:uid="{D634A6D8-9EF6-440D-ABB5-9DCA2B355EE5}"/>
-    <hyperlink ref="G18" r:id="rId47" tooltip="Manufacturer" display="'SLW-103-01-G-D" xr:uid="{FED57CA5-9773-4979-9927-B032F365B1B7}"/>
-    <hyperlink ref="J18" r:id="rId48" tooltip="Supplier" display="'SAM1088-03-ND" xr:uid="{B1B97BD8-014E-4BF1-B500-5A48D6F81745}"/>
-    <hyperlink ref="F19" r:id="rId49" tooltip="Component" display="'Samtec" xr:uid="{A867E28F-4EFC-468C-9189-2F3CB652C5FE}"/>
-    <hyperlink ref="G19" r:id="rId50" tooltip="Manufacturer" display="'SLW-115-01-G-S" xr:uid="{5092BE4A-5869-4873-8E83-158FF0E5294C}"/>
-    <hyperlink ref="J19" r:id="rId51" tooltip="Supplier" display="'SAM1089-15-ND" xr:uid="{4F49CA71-AA0A-4249-892F-2C0BA8425161}"/>
-    <hyperlink ref="F20" r:id="rId52" tooltip="Component" display="'Texas Instruments" xr:uid="{93EEFA4D-2CE9-47F3-B44A-6DE93BF6476B}"/>
-    <hyperlink ref="G20" r:id="rId53" tooltip="Manufacturer" display="'SN65HVD233D" xr:uid="{AD4938B1-E0B4-4B20-8294-E2CEF96A0067}"/>
-    <hyperlink ref="J20" r:id="rId54" tooltip="Supplier" display="'296-14639-5-ND" xr:uid="{ADA0C872-85C1-4918-B68E-9775181332D7}"/>
-    <hyperlink ref="F21" r:id="rId55" tooltip="Component" display="'Texas Instruments" xr:uid="{D298BE07-2D80-4DE9-B97D-F727B7D3F7A4}"/>
-    <hyperlink ref="G21" r:id="rId56" tooltip="Manufacturer" display="'SN74HC365PW" xr:uid="{A518407D-78D8-4EE1-8AF8-EB7B837185F1}"/>
-    <hyperlink ref="J21" r:id="rId57" tooltip="Supplier" display="'296-33932-5-ND" xr:uid="{1ACCDF0F-7D51-4450-A8E8-BA9717D06AA0}"/>
-    <hyperlink ref="F22" r:id="rId58" tooltip="Component" display="'Texas Instruments" xr:uid="{8195F2A2-E0FB-4E94-86C8-CB118617B0C6}"/>
-    <hyperlink ref="G22" r:id="rId59" tooltip="Manufacturer" display="'SN74LVC1G07DCKR" xr:uid="{D4EB5471-97EF-4989-8E76-284598A2A297}"/>
-    <hyperlink ref="J22" r:id="rId60" tooltip="Supplier" display="'296-8486-1-ND" xr:uid="{37B7FFBE-969C-448D-A943-4E7DB39954B9}"/>
-    <hyperlink ref="F23" r:id="rId61" tooltip="Component" display="'Microchip" xr:uid="{BA36AE98-2F41-4210-AC66-1886CC4A306A}"/>
-    <hyperlink ref="G23" r:id="rId62" tooltip="Manufacturer" display="'SST26VF016B-104I/SN" xr:uid="{D7D1E893-7984-4E91-8A13-F8CACFF4902E}"/>
-    <hyperlink ref="J23" r:id="rId63" tooltip="Supplier" display="'SST26VF016B-104I/SN-ND" xr:uid="{379065BD-1ED7-4662-8BEA-C44AD9C8DDB7}"/>
-    <hyperlink ref="F24" r:id="rId64" tooltip="Component" display="'ITT C&amp;K" xr:uid="{83D53E55-805D-4924-988A-4F2DC08D0ADA}"/>
-    <hyperlink ref="G24" r:id="rId65" tooltip="Manufacturer" display="'PTS830GM140SMTRLFS" xr:uid="{57D42188-82B8-4683-B56E-1AF41CA20123}"/>
-    <hyperlink ref="J24" r:id="rId66" tooltip="Supplier" display="'CKN10587CT-ND" xr:uid="{725484A1-5268-4821-982E-C6621DB70D3B}"/>
-    <hyperlink ref="F25" tooltip="Component" display="'" xr:uid="{22C79C97-BE26-49E5-B635-F3B13D472B5B}"/>
-    <hyperlink ref="G25" tooltip="Manufacturer" display="'" xr:uid="{888BD185-7E76-4DD5-BA7D-CEB8B2326E2F}"/>
-    <hyperlink ref="J25" tooltip="Supplier" display="'Samtec" xr:uid="{6B409774-17D1-4899-993A-80D77832B7AF}"/>
-    <hyperlink ref="F26" tooltip="Component" display="'" xr:uid="{AB798771-1079-4967-9657-684C41CB8148}"/>
-    <hyperlink ref="G26" tooltip="Manufacturer" display="'" xr:uid="{196E0B56-C39A-4071-899F-37EC9CF38802}"/>
-    <hyperlink ref="J26" tooltip="Supplier" display="'[NoParam], 587-3807-1-ND" xr:uid="{70DCEA57-118C-442C-B3AB-5CDE7E386D36}"/>
-    <hyperlink ref="F27" tooltip="Component" display="'" xr:uid="{27CE4556-85D7-4867-840A-235243DA561F}"/>
-    <hyperlink ref="G27" tooltip="Manufacturer" display="'" xr:uid="{0ECFAE10-1646-41AD-84B1-20DE1D91E26B}"/>
-    <hyperlink ref="J27" tooltip="Supplier" display="'[NoParam], P10.0KLCT-ND" xr:uid="{3842DBFF-7F7C-43B5-9A3D-59CF192FD70B}"/>
-    <hyperlink ref="F28" tooltip="Component" display="'" xr:uid="{FD677F0D-856C-4627-87E6-96F28FEBA126}"/>
-    <hyperlink ref="G28" tooltip="Manufacturer" display="'" xr:uid="{EE1F65FD-BD24-438D-B30F-F64051DE2395}"/>
-    <hyperlink ref="J28" tooltip="Supplier" display="'[NoParam], 541-100YCT-ND" xr:uid="{A89DB21B-3805-44DA-86F0-DB2E10E85BDB}"/>
+    <hyperlink ref="F2" tooltip="Component" display="'" xr:uid="{88997611-FE4B-4B04-B724-088B888BB1B4}"/>
+    <hyperlink ref="G2" tooltip="Manufacturer" display="'" xr:uid="{F3EB4842-5DDA-403E-9198-02DC6FCFF30A}"/>
+    <hyperlink ref="J2" tooltip="Supplier" display="'" xr:uid="{D19BB767-DA73-4D87-A994-FB5AA0E179D9}"/>
+    <hyperlink ref="F3" r:id="rId1" tooltip="Component" display="'Yageo" xr:uid="{FFF39753-5B7C-496C-88A7-DBF3B99447C4}"/>
+    <hyperlink ref="G3" r:id="rId2" tooltip="Manufacturer" display="'RC0402JR-070RL" xr:uid="{8752D1C1-995C-4CE3-97EA-C839D258C372}"/>
+    <hyperlink ref="J3" r:id="rId3" tooltip="Supplier" display="'311-0.0JRCT-ND" xr:uid="{3DDE83E4-CB0A-4B40-AAFF-8C0005D44E69}"/>
+    <hyperlink ref="F4" r:id="rId4" tooltip="Component" display="'KEMET" xr:uid="{A3F6F1D3-7FF0-4215-B9D4-5F6164D68771}"/>
+    <hyperlink ref="G4" r:id="rId5" tooltip="Manufacturer" display="'C0402C470J3RACAUTO" xr:uid="{B8D38D3E-4127-4083-B000-1DFE37EAAB8D}"/>
+    <hyperlink ref="J4" r:id="rId6" tooltip="Supplier" display="'399-17558-1-ND" xr:uid="{0EECA576-9751-41F8-B54C-8722FCE6F719}"/>
+    <hyperlink ref="F5" r:id="rId7" tooltip="Component" display="'KEMET" xr:uid="{797C8FB5-D679-48AF-9900-4A62ED9417B2}"/>
+    <hyperlink ref="G5" r:id="rId8" tooltip="Manufacturer" display="'C0402C220K4RAC7867" xr:uid="{4775D84B-B86A-4A88-ADB2-EC4700DB7DE0}"/>
+    <hyperlink ref="J5" r:id="rId9" tooltip="Supplier" display="'399-17554-1-ND" xr:uid="{2799AC72-723E-454B-A1D5-BD9F2B7D09E1}"/>
+    <hyperlink ref="F6" r:id="rId10" tooltip="Component" display="'Panasonic" xr:uid="{CF8380A1-ED81-47E4-B5CC-1A3182C41D13}"/>
+    <hyperlink ref="G6" r:id="rId11" tooltip="Manufacturer" display="'ERJ-2RKF1002X" xr:uid="{368373F8-F1DF-4DD3-8F7C-BA8F20B9FD40}"/>
+    <hyperlink ref="J6" r:id="rId12" tooltip="Supplier" display="'P10.0KLCT-ND" xr:uid="{E78506B2-1C19-4088-9DA5-9375DA60F57B}"/>
+    <hyperlink ref="F7" r:id="rId13" tooltip="Component" display="'Panasonic" xr:uid="{C6A7E471-7C26-479A-8601-8825ABC0A2C3}"/>
+    <hyperlink ref="G7" r:id="rId14" tooltip="Manufacturer" display="'ERJ-2RKF1000X" xr:uid="{298B3D32-727D-4BD2-A636-F5D174F29A8F}"/>
+    <hyperlink ref="J7" r:id="rId15" tooltip="Supplier" display="'P100LCT-ND" xr:uid="{F660B5E8-378D-4046-9CFC-FF3DCDBAB7E3}"/>
+    <hyperlink ref="F8" r:id="rId16" tooltip="Component" display="'Vishay" xr:uid="{B89C0630-74F7-47EE-8B46-1D87C006B200}"/>
+    <hyperlink ref="G8" r:id="rId17" tooltip="Manufacturer" display="'CRCW040260R4FKED" xr:uid="{07A2229D-CC80-4B59-9E45-C85AB2341CB9}"/>
+    <hyperlink ref="J8" r:id="rId18" tooltip="Supplier" display="'541-60.4LCT-ND" xr:uid="{57B3727D-0B35-4B94-9F4F-F058891DCF11}"/>
+    <hyperlink ref="F9" r:id="rId19" tooltip="Component" display="'Panasonic" xr:uid="{A5EF5160-37E1-4381-B1DB-2DF5FFE7DA52}"/>
+    <hyperlink ref="G9" r:id="rId20" tooltip="Manufacturer" display="'ERJ-2GE0R00X" xr:uid="{A28AF5D0-62AC-4E54-8B4D-38CFC68BC71E}"/>
+    <hyperlink ref="J9" r:id="rId21" tooltip="Supplier" display="'P0.0JCT-ND" xr:uid="{337DC60C-36A0-4C7F-B77D-361F06F0E1C5}"/>
+    <hyperlink ref="F10" r:id="rId22" tooltip="Component" display="'Panasonic" xr:uid="{61A85652-855C-4DD7-AB69-D9550D40E132}"/>
+    <hyperlink ref="G10" r:id="rId23" tooltip="Manufacturer" display="'ERA-2AEB472X" xr:uid="{29B1A557-3B0C-4A3E-8EDC-10488D3E6465}"/>
+    <hyperlink ref="J10" r:id="rId24" tooltip="Supplier" display="'P4.7KDCCT-ND" xr:uid="{835BF4FD-9F9F-4D53-9D8D-36A17FB50ED8}"/>
+    <hyperlink ref="F11" r:id="rId25" tooltip="Component" display="'TE Connectivity" xr:uid="{15C5326A-9C22-4C59-AB90-DB4CE85A9A05}"/>
+    <hyperlink ref="G11" r:id="rId26" tooltip="Manufacturer" display="'CRGCQ0402F330R" xr:uid="{CA431B2E-58C2-420E-8837-31625785C491}"/>
+    <hyperlink ref="J11" r:id="rId27" tooltip="Supplier" display="'A129621CT-ND" xr:uid="{E7E79719-D2B6-4CCA-B4E9-EF46C6745ADF}"/>
+    <hyperlink ref="F12" r:id="rId28" tooltip="Component" display="'Yageo" xr:uid="{1A01E39C-CF24-4BE1-A40C-A7831B70C530}"/>
+    <hyperlink ref="G12" r:id="rId29" tooltip="Manufacturer" display="'AC0402FR-0730KL" xr:uid="{222B0099-3CA0-43F8-9B77-7B9664A0CE39}"/>
+    <hyperlink ref="J12" r:id="rId30" tooltip="Supplier" display="'YAG3474CT-ND" xr:uid="{6DFC2F77-0F38-46FE-8370-588EBB76BB64}"/>
+    <hyperlink ref="F13" r:id="rId31" tooltip="Component" display="'TDK" xr:uid="{F99326C6-0EA1-434B-B350-E0521FC68A27}"/>
+    <hyperlink ref="G13" r:id="rId32" tooltip="Manufacturer" display="'MLZ1608N100LTD25" xr:uid="{3D15A8AE-E18A-4D69-95AB-64452A904DD6}"/>
+    <hyperlink ref="J13" r:id="rId33" tooltip="Supplier" display="'445-17067-1-ND" xr:uid="{1345B5CF-B284-4D15-85C0-8A80B808CCFD}"/>
+    <hyperlink ref="F14" r:id="rId34" tooltip="Component" display="'Murata" xr:uid="{A56EB303-196F-4159-9FD3-1AAFE6E09D62}"/>
+    <hyperlink ref="G14" r:id="rId35" tooltip="Manufacturer" display="'GCM21BR70J106KE22K" xr:uid="{132020E3-4312-45D2-8D11-0522E9D0E71C}"/>
+    <hyperlink ref="J14" r:id="rId36" tooltip="Supplier" display="'490-14361-1-ND" xr:uid="{06DDE95D-D5DC-4EFD-A032-3FAFAB530CB7}"/>
+    <hyperlink ref="F15" r:id="rId37" tooltip="Component" display="'Abracon" xr:uid="{DC107E8E-18ED-4ED8-A0B9-C99445B5217F}"/>
+    <hyperlink ref="G15" r:id="rId38" tooltip="Manufacturer" display="'ABM3B-8.000MHZ-10-D-1-G-T" xr:uid="{1947C7A3-F91F-4213-838B-7B45B4219C83}"/>
+    <hyperlink ref="J15" r:id="rId39" tooltip="Supplier" display="'535-13456-1-ND" xr:uid="{5BD233F0-D723-4703-B8CF-926B6542A87E}"/>
+    <hyperlink ref="F16" r:id="rId40" tooltip="Component" display="'Microchip / Atmel" xr:uid="{4305A646-F678-42A0-B8BD-D1DF2E137648}"/>
+    <hyperlink ref="G16" r:id="rId41" tooltip="Manufacturer" display="'ATMEGA64M1-AU" xr:uid="{9643B9EA-5E4B-46D4-BDA6-8D6979F7AD44}"/>
+    <hyperlink ref="J16" r:id="rId42" tooltip="Supplier" display="'ATMEGA64M1-AU-ND" xr:uid="{824EF656-0C11-4FCC-9F25-2F0CB9F84650}"/>
+    <hyperlink ref="F17" r:id="rId43" tooltip="Component" display="'Maxim" xr:uid="{B2D5DB2A-9ED5-4F73-AAB2-0A98DAD96D86}"/>
+    <hyperlink ref="G17" r:id="rId44" tooltip="Manufacturer" display="'DS3234SN#T&amp;R" xr:uid="{69F2635F-A3CB-4120-88B0-3689559C68C5}"/>
+    <hyperlink ref="J17" r:id="rId45" tooltip="Supplier" display="'DS3234SN#T&amp;RCT-ND" xr:uid="{7C6D7921-BF16-48B2-B120-287D8EF7A119}"/>
+    <hyperlink ref="F18" r:id="rId46" tooltip="Component" display="'NXP USA" xr:uid="{B5138A54-AA5C-4969-900D-E370B3EE58D0}"/>
+    <hyperlink ref="G18" r:id="rId47" tooltip="Manufacturer" display="'SC18IS600IPW/S8HP" xr:uid="{BB375583-E151-4576-B67B-CEE300BB9901}"/>
+    <hyperlink ref="J18" r:id="rId48" tooltip="Supplier" display="'568-13690-1-ND" xr:uid="{84A99EA4-11EB-497B-8C53-9E4E36504270}"/>
+    <hyperlink ref="F19" r:id="rId49" tooltip="Component" display="'Samtec" xr:uid="{91C47081-F5B1-4D8D-AA93-7899CFD9D677}"/>
+    <hyperlink ref="G19" r:id="rId50" tooltip="Manufacturer" display="'SLW-102-01-G-D" xr:uid="{9F199592-41B5-4F4F-964E-2A44496897B6}"/>
+    <hyperlink ref="J19" r:id="rId51" tooltip="Supplier" display="'SAM1088-02-ND" xr:uid="{371A7CC0-1DF4-415C-8683-641A48C5C731}"/>
+    <hyperlink ref="F20" r:id="rId52" tooltip="Component" display="'Samtec" xr:uid="{61C31BAE-7BE5-4F85-9696-6692DAA7ACDF}"/>
+    <hyperlink ref="G20" r:id="rId53" tooltip="Manufacturer" display="'SLW-103-01-G-D" xr:uid="{F8FF2A15-B887-4902-B72E-823BA84DFA3C}"/>
+    <hyperlink ref="J20" r:id="rId54" tooltip="Supplier" display="'SAM1088-03-ND" xr:uid="{0C5C3B94-E982-4D25-9A3B-28B910654FEA}"/>
+    <hyperlink ref="F21" r:id="rId55" tooltip="Component" display="'Samtec" xr:uid="{F9392BBB-26A7-46D1-B587-2DD2C125D700}"/>
+    <hyperlink ref="G21" r:id="rId56" tooltip="Manufacturer" display="'SLW-115-01-G-S" xr:uid="{76D5C168-FCEB-4FB9-8377-56C4C83CC0C2}"/>
+    <hyperlink ref="J21" r:id="rId57" tooltip="Supplier" display="'SAM1089-15-ND" xr:uid="{A95E0663-E214-43BE-8B5E-C733C8F0713C}"/>
+    <hyperlink ref="F22" r:id="rId58" tooltip="Component" display="'Texas Instruments" xr:uid="{55F37D03-1D8C-4B49-BB84-1149391AAD7B}"/>
+    <hyperlink ref="G22" r:id="rId59" tooltip="Manufacturer" display="'SN65HVD233D" xr:uid="{EDFADCC5-B557-4E6D-B139-41033C5E12F2}"/>
+    <hyperlink ref="J22" r:id="rId60" tooltip="Supplier" display="'296-14639-5-ND" xr:uid="{5AB0BC08-7032-47D2-B74D-6A89BED847BF}"/>
+    <hyperlink ref="F23" r:id="rId61" tooltip="Component" display="'Texas Instruments" xr:uid="{5AC668EA-8F82-440D-B296-454B7C5BE02D}"/>
+    <hyperlink ref="G23" r:id="rId62" tooltip="Manufacturer" display="'SN74HC365PW" xr:uid="{6404615B-D96E-45F1-BDFD-49672B53502B}"/>
+    <hyperlink ref="J23" r:id="rId63" tooltip="Supplier" display="'296-33932-5-ND" xr:uid="{20C4DCDF-ACAC-4363-865E-45A43F1021F2}"/>
+    <hyperlink ref="F24" r:id="rId64" tooltip="Component" display="'Texas Instruments" xr:uid="{A20255CE-368E-4AD0-9C5E-4344A7C8426C}"/>
+    <hyperlink ref="G24" r:id="rId65" tooltip="Manufacturer" display="'SN74LVC1G07DCKR" xr:uid="{BDA4328F-04BB-4505-B40C-873BE96A2E5B}"/>
+    <hyperlink ref="J24" r:id="rId66" tooltip="Supplier" display="'296-8486-1-ND" xr:uid="{9F6D064C-4DF9-4280-B407-5FB6BB227B24}"/>
+    <hyperlink ref="F25" r:id="rId67" tooltip="Component" display="'Microchip" xr:uid="{6A042C65-500E-49E5-A693-AC47D626344B}"/>
+    <hyperlink ref="G25" r:id="rId68" tooltip="Manufacturer" display="'SST26VF016B-104I/SN" xr:uid="{4473F25C-4379-47FA-8CF9-A3D0171F9AD0}"/>
+    <hyperlink ref="J25" r:id="rId69" tooltip="Supplier" display="'SST26VF016B-104I/SN-ND" xr:uid="{8B9C85B2-DF29-4746-AFD6-AAB9F66CAA72}"/>
+    <hyperlink ref="F26" r:id="rId70" tooltip="Component" display="'ITT C&amp;K" xr:uid="{13C49897-A89E-4533-BD26-57DC2C287197}"/>
+    <hyperlink ref="G26" r:id="rId71" tooltip="Manufacturer" display="'PTS830GM140SMTRLFS" xr:uid="{A962C740-5A9B-4DA8-8161-0AA1B5C174B5}"/>
+    <hyperlink ref="J26" r:id="rId72" tooltip="Supplier" display="'CKN10587CT-ND" xr:uid="{39761D76-81C1-46EE-8C79-F74869C1F9E5}"/>
+    <hyperlink ref="F27" r:id="rId73" tooltip="Component" display="'ITT C&amp;K" xr:uid="{5EBEECBD-4279-4A99-AED4-8156C4D0653C}"/>
+    <hyperlink ref="G27" r:id="rId74" tooltip="Manufacturer" display="'JS202011AQN" xr:uid="{1D664FA1-E2C8-4F57-B110-C23C590EFCAA}"/>
+    <hyperlink ref="J27" r:id="rId75" tooltip="Supplier" display="'611-JS202011AQN" xr:uid="{5DAE256E-F285-42D2-B696-839077400AC9}"/>
+    <hyperlink ref="F28" tooltip="Component" display="'" xr:uid="{21CFBA13-F8FC-4843-944A-64CD90AB2A5A}"/>
+    <hyperlink ref="G28" tooltip="Manufacturer" display="'" xr:uid="{FE8CF9B5-6A44-4F95-A420-C60111112548}"/>
+    <hyperlink ref="J28" tooltip="Supplier" display="'Samtec" xr:uid="{DAB147D0-F620-4027-86E0-AC248DB5D92D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
</xml_diff>